<commit_message>
✨ Update TAS form.
</commit_message>
<xml_diff>
--- a/LF/Pre TAS/lf_pretas_1_site.xlsx
+++ b/LF/Pre TAS/lf_pretas_1_site.xlsx
@@ -109,12 +109,6 @@
     <t>Select your district</t>
   </si>
   <si>
-    <t>c_site</t>
-  </si>
-  <si>
-    <t>Is the Cluster a School or Community</t>
-  </si>
-  <si>
     <t>c_cluster_name</t>
   </si>
   <si>
@@ -199,9 +193,6 @@
     <t>Sélectionner le district</t>
   </si>
   <si>
-    <t>La grappe est-il une école ou une communauté</t>
-  </si>
-  <si>
     <t>Entrer le nom de la grappe</t>
   </si>
   <si>
@@ -362,6 +353,15 @@
   </si>
   <si>
     <t>pretas_lf_1_site</t>
+  </si>
+  <si>
+    <t>c_site_type</t>
+  </si>
+  <si>
+    <t>Is it a sentinel site or a spot-check site</t>
+  </si>
+  <si>
+    <t>Est-ce un site sentinelle ou un site de control ponctuelle</t>
   </si>
 </sst>
 </file>
@@ -800,10 +800,10 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15:E16"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -840,10 +840,10 @@
         <v>16</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G1" s="14" t="s">
         <v>6</v>
@@ -855,7 +855,7 @@
         <v>17</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K1" s="14" t="s">
         <v>8</v>
@@ -878,7 +878,7 @@
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>19</v>
@@ -890,25 +890,25 @@
         <v>21</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
@@ -916,7 +916,7 @@
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>22</v>
@@ -926,7 +926,7 @@
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="8"/>
@@ -936,14 +936,14 @@
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
     </row>
     <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>24</v>
@@ -953,7 +953,7 @@
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="8"/>
@@ -962,27 +962,27 @@
       <c r="J4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>26</v>
+        <v>108</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="8"/>
@@ -992,7 +992,7 @@
       <c r="K5" s="4"/>
       <c r="L5" s="3"/>
       <c r="M5" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -1000,22 +1000,22 @@
     </row>
     <row r="6" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="E6" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
@@ -1024,7 +1024,7 @@
       <c r="K6" s="4"/>
       <c r="L6" s="3"/>
       <c r="M6" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
@@ -1032,33 +1032,33 @@
     </row>
     <row r="7" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
@@ -1066,29 +1066,29 @@
     </row>
     <row r="8" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
@@ -1096,17 +1096,17 @@
     </row>
     <row r="9" spans="1:16" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1116,7 +1116,7 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
@@ -1124,17 +1124,17 @@
     </row>
     <row r="10" spans="1:16" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="8"/>
@@ -1144,7 +1144,7 @@
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
@@ -1152,93 +1152,93 @@
     </row>
     <row r="11" spans="1:16" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F11" s="13"/>
       <c r="H11" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F12" s="13"/>
       <c r="M12" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B13" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>45</v>
-      </c>
       <c r="E13" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
@@ -1246,13 +1246,13 @@
     </row>
     <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
@@ -1270,7 +1270,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1292,159 +1292,159 @@
         <v>15</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
         <v>81</v>
-      </c>
-      <c r="C7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" t="s">
         <v>82</v>
-      </c>
-      <c r="C8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D8" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" t="s">
         <v>80</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" t="s">
         <v>83</v>
-      </c>
-      <c r="C9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" t="s">
         <v>92</v>
-      </c>
-      <c r="B10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C10" t="s">
-        <v>93</v>
-      </c>
-      <c r="D10" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1486,10 +1486,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C2">
         <v>20200402</v>

</xml_diff>

<commit_message>
🎨 renamed some variables.
</commit_message>
<xml_diff>
--- a/LF/Pre TAS/lf_pretas_1_site.xlsx
+++ b/LF/Pre TAS/lf_pretas_1_site.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbandubad\Repositories\generic-espen-collect-form\LF\Pre TAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\generic-espen-collect-form\LF\Pre TAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFB529D-D493-47DF-8D7F-4973846BC6E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="25785" windowHeight="13980" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -124,15 +125,9 @@
     <t>Name of Village Leader or Head Teacher</t>
   </si>
   <si>
-    <t>c_clusterID1</t>
-  </si>
-  <si>
     <t>Enter Cluster ID</t>
   </si>
   <si>
-    <t>c_clusterID2</t>
-  </si>
-  <si>
     <t>Enter Cluster ID again</t>
   </si>
   <si>
@@ -163,9 +158,6 @@
     <t>GPS coordinates are easier to collect outside. 2 min timeout</t>
   </si>
   <si>
-    <t>c_ClusterNotes</t>
-  </si>
-  <si>
     <t>Additional notes to add?</t>
   </si>
   <si>
@@ -337,9 +329,6 @@
     <t>Le code doit être un nombre à deux chiffres entre 9 et 91</t>
   </si>
   <si>
-    <t>. = ${c_clusterID1}</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -362,12 +351,24 @@
   </si>
   <si>
     <t>Est-ce un site sentinelle ou un site de control ponctuelle</t>
+  </si>
+  <si>
+    <t>c_cluster_id1</t>
+  </si>
+  <si>
+    <t>c_cluster_id2</t>
+  </si>
+  <si>
+    <t>. = ${c_cluster_id1}</t>
+  </si>
+  <si>
+    <t>c_cluster_notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -796,14 +797,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -840,10 +841,10 @@
         <v>16</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G1" s="14" t="s">
         <v>6</v>
@@ -855,7 +856,7 @@
         <v>17</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K1" s="14" t="s">
         <v>8</v>
@@ -878,7 +879,7 @@
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>19</v>
@@ -890,25 +891,25 @@
         <v>21</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
@@ -916,7 +917,7 @@
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>22</v>
@@ -926,7 +927,7 @@
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="8"/>
@@ -936,14 +937,14 @@
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
     </row>
     <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>24</v>
@@ -953,7 +954,7 @@
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="8"/>
@@ -962,27 +963,27 @@
       <c r="J4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="8"/>
@@ -992,7 +993,7 @@
       <c r="K5" s="4"/>
       <c r="L5" s="3"/>
       <c r="M5" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -1000,7 +1001,7 @@
     </row>
     <row r="6" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>26</v>
@@ -1012,10 +1013,10 @@
         <v>28</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
@@ -1024,7 +1025,7 @@
       <c r="K6" s="4"/>
       <c r="L6" s="3"/>
       <c r="M6" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
@@ -1032,33 +1033,33 @@
     </row>
     <row r="7" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
@@ -1066,29 +1067,29 @@
     </row>
     <row r="8" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="4" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
@@ -1096,7 +1097,7 @@
     </row>
     <row r="9" spans="1:16" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>29</v>
@@ -1106,7 +1107,7 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1116,7 +1117,7 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
@@ -1124,17 +1125,17 @@
     </row>
     <row r="10" spans="1:16" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="8"/>
@@ -1144,7 +1145,7 @@
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
@@ -1152,93 +1153,93 @@
     </row>
     <row r="11" spans="1:16" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F11" s="13"/>
       <c r="H11" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F12" s="13"/>
       <c r="M12" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B13" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>43</v>
-      </c>
       <c r="E13" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>44</v>
+        <v>110</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
@@ -1246,13 +1247,13 @@
     </row>
     <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
@@ -1265,7 +1266,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1292,163 +1293,163 @@
         <v>15</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" t="s">
         <v>78</v>
-      </c>
-      <c r="C7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" t="s">
         <v>79</v>
-      </c>
-      <c r="C8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" t="s">
         <v>77</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" t="s">
         <v>80</v>
-      </c>
-      <c r="C9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" t="s">
         <v>89</v>
-      </c>
-      <c r="B10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A14:C59">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:C59">
     <sortCondition ref="B14:B59"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1456,7 +1457,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1486,10 +1487,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C2">
         <v>20200402</v>

</xml_diff>